<commit_message>
se realiza la prueba 4
</commit_message>
<xml_diff>
--- a/src/test/resources/dataExcel/DatosDePrueba.xlsx
+++ b/src/test/resources/dataExcel/DatosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crown\Desktop\PageObjectModel\src\test\resources\dataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AB3B9D-69F4-4BBD-8F94-8A1C55870A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863C7033-4E9B-4A07-B621-B2A0E2994408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="2760" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>CP004</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>CP005</t>
   </si>
@@ -92,6 +89,15 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>CP004_buscarPorNombre</t>
+  </si>
+  <si>
+    <t>Venta cancelada</t>
+  </si>
+  <si>
+    <t>rodolfo</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -229,21 +235,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -282,11 +273,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -572,7 +565,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -581,44 +574,45 @@
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -626,17 +620,17 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -644,17 +638,17 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -662,35 +656,43 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="8" t="s">
-        <v>1</v>
+      <c r="A6" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>5456</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1">

</xml_diff>

<commit_message>
se termina los casos de pruebas
</commit_message>
<xml_diff>
--- a/src/test/resources/dataExcel/DatosDePrueba.xlsx
+++ b/src/test/resources/dataExcel/DatosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crown\Desktop\PageObjectModel\src\test\resources\dataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863C7033-4E9B-4A07-B621-B2A0E2994408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2131764-7069-4D39-B577-2071894F097C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2760" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="2760" windowWidth="25170" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosCP" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
-  <si>
-    <t>CP005</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Dato 1</t>
   </si>
@@ -55,15 +52,6 @@
     <t>hola</t>
   </si>
   <si>
-    <t>hla</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>ef</t>
-  </si>
-  <si>
     <t>CP001_ingresoLogin</t>
   </si>
   <si>
@@ -98,6 +86,12 @@
   </si>
   <si>
     <t>rodolfo</t>
+  </si>
+  <si>
+    <t>CP005_datosCliente</t>
+  </si>
+  <si>
+    <t>TERMINE JAJAJAJAJAJAJAJA</t>
   </si>
 </sst>
 </file>
@@ -131,7 +125,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,14 +138,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -175,31 +163,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -212,9 +185,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -227,59 +198,23 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,72 +500,74 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>18</v>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -638,17 +575,17 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -656,45 +593,47 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>22</v>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1">
-        <v>5456</v>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G6" s="1">
+        <v>962545885</v>
+      </c>
       <c r="H6" s="1">
         <v>555</v>
       </c>

</xml_diff>

<commit_message>
Se termina curso de selenium
</commit_message>
<xml_diff>
--- a/src/test/resources/dataExcel/DatosDePrueba.xlsx
+++ b/src/test/resources/dataExcel/DatosDePrueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crown\Desktop\PageObjectModel\src\test\resources\dataExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crown\Desktop\Trabajos de Repaso\PageObjectModel\src\test\resources\dataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2131764-7069-4D39-B577-2071894F097C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C942E2B2-717E-4DA7-8704-39C4FCC7508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="2760" windowWidth="25170" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>